<commit_message>
Ran rate Accuracy on all projects
</commit_message>
<xml_diff>
--- a/sample_tests.xlsx
+++ b/sample_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SegmentUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00404960-3FFD-401F-A186-358F15B7A9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4949B14-1FD1-4DAC-89D7-DDB508060CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16305" yWindow="14040" windowWidth="16410" windowHeight="14145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t>Other Tests</t>
   </si>
   <si>
-    <t>Pass Rate</t>
-  </si>
-  <si>
     <t>aquafun</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>% Pass</t>
+  </si>
+  <si>
+    <t>Average Pass Rate</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.4166666666666665</c:v>
+                  <c:v>2.3333333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,7 +624,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.4166666666666665</c:v>
+                  <c:v>2.3333333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1170,7 +1170,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.3809523809523809</c:v>
+                  <c:v>2.3333333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1259,7 +1259,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.4761904761904763</c:v>
+                  <c:v>2.4285714285714284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,7 +1578,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pass Rate</c:v>
+                  <c:v>Average Pass Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1631,7 +1631,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pass Rate</c:v>
+                  <c:v>Average Pass Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1684,7 +1684,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pass Rate</c:v>
+                  <c:v>Average Pass Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1737,7 +1737,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pass Rate</c:v>
+                  <c:v>Average Pass Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2068,7 +2068,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average Ranking</c:v>
+                  <c:v>Average Pass Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2121,7 +2121,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average Ranking</c:v>
+                  <c:v>Average Pass Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2174,7 +2174,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average Ranking</c:v>
+                  <c:v>Average Pass Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2227,7 +2227,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average Ranking</c:v>
+                  <c:v>Average Pass Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5042,8 +5042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:E32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5258,10 +5258,10 @@
         <v>1</v>
       </c>
       <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
         <v>3</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -5283,7 +5283,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1">
         <f>AVERAGE(B4:B15)</f>
@@ -5295,11 +5295,11 @@
       </c>
       <c r="D17" s="1">
         <f>AVERAGE(D4:D15)</f>
-        <v>2.4166666666666665</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="E17" s="1">
         <f>AVERAGE(E4:E15)</f>
-        <v>2.4166666666666665</v>
+        <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -5331,7 +5331,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -5365,7 +5365,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -5382,7 +5382,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -5399,7 +5399,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -5416,7 +5416,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -5433,7 +5433,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -5450,7 +5450,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -5467,7 +5467,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>4</v>
@@ -5484,7 +5484,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1">
         <f>AVERAGE(B21:B29, B4:B15)</f>
@@ -5496,11 +5496,11 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
-        <v>2.3809523809523809</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>2.4761904761904763</v>
+        <v>2.4285714285714284</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5510,6 +5510,16 @@
       <c r="E32" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B4:E15 B21:E29">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5519,13 +5529,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7E62FB-99A1-4A88-9128-20EC8B40431C}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
@@ -5535,10 +5545,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -5558,7 +5568,7 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -5818,7 +5828,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2">
         <f>AVERAGE(B4:B15)</f>
@@ -5861,12 +5871,12 @@
         <v>16</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -5887,7 +5897,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -5908,7 +5918,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5929,7 +5939,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -5950,7 +5960,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -5971,7 +5981,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -5992,7 +6002,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -6013,7 +6023,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -6034,7 +6044,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -6055,7 +6065,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2">
         <f>AVERAGE(B21:B29, B4:B15)</f>
@@ -6075,6 +6085,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B4:E15 B21:E29">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added thesis graphics file
</commit_message>
<xml_diff>
--- a/sample_tests.xlsx
+++ b/sample_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SegmentUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4949B14-1FD1-4DAC-89D7-DDB508060CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF329C7-E529-4C3D-A2FC-A10EA1B760FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking" sheetId="1" r:id="rId1"/>
@@ -5043,7 +5043,7 @@
   <dimension ref="A3:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added to excel file
</commit_message>
<xml_diff>
--- a/sample_tests.xlsx
+++ b/sample_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SegmentUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78DD519-0921-49B2-AF9A-7DFD12FE6C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7F5BEB-0BB8-4C3E-8A23-14470DDB47E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16305" yWindow="14040" windowWidth="16410" windowHeight="14145" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="43">
   <si>
     <t>adventure</t>
   </si>
@@ -161,6 +161,15 @@
   <si>
     <t>Time Increase over Zero-shot</t>
   </si>
+  <si>
+    <t>Average Time</t>
+  </si>
+  <si>
+    <t>Zero-Shot</t>
+  </si>
+  <si>
+    <t>Percent Increase</t>
+  </si>
 </sst>
 </file>
 
@@ -209,13 +218,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9506,17 +9516,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB29B34-CF1B-D945-9D6F-06FCC2222DED}">
   <dimension ref="A3:E32"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -9815,6 +9825,11 @@
       <c r="E21" s="2">
         <v>0.75</v>
       </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B31" s="1"/>
@@ -10514,8 +10529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7E62FB-99A1-4A88-9128-20EC8B40431C}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:P38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11088,18 +11103,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CAC04A-32BE-4E8D-B040-C961AC1E9CE4}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.36328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -11151,10 +11166,21 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>7.26</v>
+        <v>9.49</v>
+      </c>
+      <c r="C3">
+        <v>693.46</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="0">C3+B3</f>
+        <v>702.95</v>
       </c>
       <c r="F3">
         <v>47.06</v>
+      </c>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H6" si="1">((D3 - F3) / F3)</f>
+        <v>13.937314067148323</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -11162,10 +11188,21 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>6.44</v>
+        <v>8.36</v>
+      </c>
+      <c r="C4">
+        <v>223.22</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>231.57999999999998</v>
       </c>
       <c r="F4">
         <v>42.69</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="1"/>
+        <v>4.4246896228624966</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -11173,10 +11210,21 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>10.14</v>
+        <v>8.82</v>
+      </c>
+      <c r="C5">
+        <v>326.43</v>
+      </c>
+      <c r="D5">
+        <f>C5+B5</f>
+        <v>335.25</v>
       </c>
       <c r="F5">
         <v>48.08</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="1"/>
+        <v>5.9727537437603999</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -11184,10 +11232,59 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>10.88</v>
+        <v>10.68</v>
+      </c>
+      <c r="C6">
+        <v>625.02</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>635.69999999999993</v>
       </c>
       <c r="F6">
         <v>65.459999999999994</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="1"/>
+        <v>8.7112740604949579</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <f>AVERAGE(B2:B6)</f>
+        <v>8.7159999999999993</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE(C2:C6)</f>
+        <v>424.53600000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="1">
+        <f>AVERAGE(F2:F6)</f>
+        <v>52.373999999999988</v>
+      </c>
+      <c r="C10" s="1">
+        <f>AVERAGE(D2:D6)</f>
+        <v>433.25199999999995</v>
+      </c>
+      <c r="D10" s="6">
+        <f>((C10 - B10) / B10)</f>
+        <v>7.2722725016229441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>